<commit_message>
Added Cosine interpolation to Driver
</commit_message>
<xml_diff>
--- a/doc/Interpolation.xlsx
+++ b/doc/Interpolation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tompit-my.sharepoint.com/personal/ales_hotko_tompit_net/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Development\MathExtended.Interpolation.old\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{420954F6-8BB1-413B-9DB0-830943815021}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39FA407-824A-43A4-9112-43D548069C55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0ECB7FB-992C-46C1-9D13-B1435819DD79}"/>
   </bookViews>
@@ -31,15 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>X</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Spline</t>
   </si>
   <si>
     <t>Linear</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Cosine</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,37 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -118,6 +151,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -130,324 +174,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$112</c:f>
+              <c:f>Sheet1!$B$2:$B$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="111"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.9000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.4</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6.6</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>8.1</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>8.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>9.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>10.1</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>10.4</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>10.6</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>10.8</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>10.9</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$112</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="111"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -757,13 +489,24 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C07B-4EFA-BA98-F108A461C8E4}"/>
+              <c16:uniqueId val="{00000001-ECDE-4B05-B606-451D5D2CBCDB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Spline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -776,324 +519,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$112</c:f>
+              <c:f>Sheet1!$C$2:$C$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="111"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.9000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.4</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5.9</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.3</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.4</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6.6</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>6.8</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>7.3</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>8.1</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>8.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>8.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>8.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>8.9</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>9.1</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>9.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>9.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>9.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>9.9</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>10.1</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>10.3</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>10.4</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>10.6</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>10.7</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>10.8</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>10.9</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$112</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="111"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1403,7 +834,352 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C07B-4EFA-BA98-F108A461C8E4}"/>
+              <c16:uniqueId val="{00000002-ECDE-4B05-B606-451D5D2CBCDB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cosine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1469999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2280000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.327</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.573</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.7189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.879</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.052</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0730000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.7649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.2350000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.4690000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.9269999999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.1479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.7629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.9480000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.1210000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.2809999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.4269999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.5579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.673</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.7720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.8529999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.9169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.9630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.9909999999999997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.99</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.96</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.91</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.84</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.7530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.649</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.5289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.3959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.0940000000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.76</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.5869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.4130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.07</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.9059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.6040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.4710000000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.351</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.2469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.16</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.0469999999999997</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.1849999999999996</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.4139999999999997</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.7279999999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.1210000000000004</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.5869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.117</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.3260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.9830000000000005</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.6590000000000007</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10.340999999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>11.016999999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>11.673999999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>12.882999999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>13.413</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>13.879</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>14.272</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>14.586</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>14.815</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>14.952999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>14.909000000000001</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>14.647</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>14.237</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>13.722</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>12.577999999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>12.063000000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>11.653</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>11.391</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-ECDE-4B05-B606-451D5D2CBCDB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1416,17 +1192,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="682218336"/>
-        <c:axId val="682215384"/>
+        <c:axId val="437657208"/>
+        <c:axId val="437657536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="682218336"/>
+        <c:axId val="437657208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1463,7 +1238,7 @@
             <a:endParaRPr lang="en-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="682215384"/>
+        <c:crossAx val="437657536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1471,7 +1246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="682215384"/>
+        <c:axId val="437657536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1297,7 @@
             <a:endParaRPr lang="en-SI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="682218336"/>
+        <c:crossAx val="437657208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2170,22 +1945,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
+      <xdr:colOff>447674</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{416E6A1E-FFFE-4193-837D-D749E152CB32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9982A2A9-6468-4FFB-BF66-06FDC0C204A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,26 +2278,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F21F3-5072-4CDB-BA8E-DF3C6E754D6A}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C102"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2532,8 +2310,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -2543,8 +2324,11 @@
       <c r="C3">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2.0089999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -2554,8 +2338,11 @@
       <c r="C4">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2.0369999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -2565,8 +2352,11 @@
       <c r="C5">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2.0830000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -2576,8 +2366,11 @@
       <c r="C6">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2.1469999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -2587,8 +2380,11 @@
       <c r="C7">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>2.2280000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.6</v>
       </c>
@@ -2598,8 +2394,11 @@
       <c r="C8">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2.327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.7</v>
       </c>
@@ -2609,8 +2408,11 @@
       <c r="C9">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2.4420000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.8</v>
       </c>
@@ -2620,8 +2422,11 @@
       <c r="C10">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2.573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.9</v>
       </c>
@@ -2631,8 +2436,11 @@
       <c r="C11">
         <v>3.35</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2.7189999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2642,8 +2450,11 @@
       <c r="C12">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2.879</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.1</v>
       </c>
@@ -2653,8 +2464,11 @@
       <c r="C13">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>3.052</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -2664,8 +2478,11 @@
       <c r="C14">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>3.2370000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.2999999999999998</v>
       </c>
@@ -2675,8 +2492,11 @@
       <c r="C15">
         <v>3.95</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>3.4329999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.4</v>
       </c>
@@ -2686,8 +2506,11 @@
       <c r="C16">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3.6379999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.5</v>
       </c>
@@ -2697,8 +2520,11 @@
       <c r="C17">
         <v>4.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>3.8519999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2.6</v>
       </c>
@@ -2708,8 +2534,11 @@
       <c r="C18">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>4.0730000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.7</v>
       </c>
@@ -2719,8 +2548,11 @@
       <c r="C19">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.8</v>
       </c>
@@ -2730,8 +2562,11 @@
       <c r="C20">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>4.5309999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2.9</v>
       </c>
@@ -2741,8 +2576,11 @@
       <c r="C21">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>4.7649999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2752,8 +2590,11 @@
       <c r="C22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3.1</v>
       </c>
@@ -2763,8 +2604,11 @@
       <c r="C23">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5.2350000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -2774,8 +2618,11 @@
       <c r="C24">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5.4690000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.3</v>
       </c>
@@ -2785,8 +2632,11 @@
       <c r="C25">
         <v>5.45</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.4</v>
       </c>
@@ -2796,8 +2646,11 @@
       <c r="C26">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>5.9269999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3.5</v>
       </c>
@@ -2807,8 +2660,11 @@
       <c r="C27">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>6.1479999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3.6</v>
       </c>
@@ -2818,8 +2674,11 @@
       <c r="C28">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>6.3620000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3.7</v>
       </c>
@@ -2829,8 +2688,11 @@
       <c r="C29">
         <v>6.05</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>6.5670000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3.8</v>
       </c>
@@ -2840,8 +2702,11 @@
       <c r="C30">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>6.7629999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3.9</v>
       </c>
@@ -2851,8 +2716,11 @@
       <c r="C31">
         <v>6.35</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>6.9480000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2862,8 +2730,11 @@
       <c r="C32">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>7.1210000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.0999999999999996</v>
       </c>
@@ -2873,8 +2744,11 @@
       <c r="C33">
         <v>6.65</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>7.2809999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4.2</v>
       </c>
@@ -2884,8 +2758,11 @@
       <c r="C34">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>7.4269999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4.3</v>
       </c>
@@ -2895,8 +2772,11 @@
       <c r="C35">
         <v>6.95</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>7.5579999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4.4000000000000004</v>
       </c>
@@ -2906,8 +2786,11 @@
       <c r="C36">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>7.673</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4.5</v>
       </c>
@@ -2917,8 +2800,11 @@
       <c r="C37">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>7.7720000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4.5999999999999996</v>
       </c>
@@ -2928,8 +2814,11 @@
       <c r="C38">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>7.8529999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4.7</v>
       </c>
@@ -2939,8 +2828,11 @@
       <c r="C39">
         <v>7.55</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>7.9169999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4.8</v>
       </c>
@@ -2950,8 +2842,11 @@
       <c r="C40">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>7.9630000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4.9000000000000004</v>
       </c>
@@ -2961,8 +2856,11 @@
       <c r="C41">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>7.9909999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2972,8 +2870,11 @@
       <c r="C42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.0999999999999996</v>
       </c>
@@ -2983,8 +2884,11 @@
       <c r="C43">
         <v>7.8890000000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.2</v>
       </c>
@@ -2994,8 +2898,11 @@
       <c r="C44">
         <v>7.7779999999999996</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.3</v>
       </c>
@@ -3005,8 +2912,11 @@
       <c r="C45">
         <v>7.6669999999999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.4</v>
       </c>
@@ -3016,8 +2926,11 @@
       <c r="C46">
         <v>7.556</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.5</v>
       </c>
@@ -3027,8 +2940,11 @@
       <c r="C47">
         <v>7.444</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>7.7530000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5.6</v>
       </c>
@@ -3038,8 +2954,11 @@
       <c r="C48">
         <v>7.3330000000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>7.649</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.7</v>
       </c>
@@ -3049,8 +2968,11 @@
       <c r="C49">
         <v>7.2220000000000004</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>7.5289999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.8</v>
       </c>
@@ -3060,8 +2982,11 @@
       <c r="C50">
         <v>7.1109999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>7.3959999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.9</v>
       </c>
@@ -3071,8 +2996,11 @@
       <c r="C51">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -3082,8 +3010,11 @@
       <c r="C52">
         <v>6.8890000000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>7.0940000000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6.1</v>
       </c>
@@ -3093,8 +3024,11 @@
       <c r="C53">
         <v>6.7779999999999996</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6.2</v>
       </c>
@@ -3104,8 +3038,11 @@
       <c r="C54">
         <v>6.6669999999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6.3</v>
       </c>
@@ -3115,8 +3052,11 @@
       <c r="C55">
         <v>6.556</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>6.5869999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6.4</v>
       </c>
@@ -3126,8 +3066,11 @@
       <c r="C56">
         <v>6.444</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>6.4130000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6.5</v>
       </c>
@@ -3137,8 +3080,11 @@
       <c r="C57">
         <v>6.3330000000000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6.6</v>
       </c>
@@ -3148,8 +3094,11 @@
       <c r="C58">
         <v>6.2220000000000004</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6.7</v>
       </c>
@@ -3159,8 +3108,11 @@
       <c r="C59">
         <v>6.1109999999999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>5.9059999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6.8</v>
       </c>
@@ -3170,8 +3122,11 @@
       <c r="C60">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6.9</v>
       </c>
@@ -3181,8 +3136,11 @@
       <c r="C61">
         <v>5.8890000000000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>5.6040000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7</v>
       </c>
@@ -3192,8 +3150,11 @@
       <c r="C62">
         <v>5.7779999999999996</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>5.4710000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7.1</v>
       </c>
@@ -3203,8 +3164,11 @@
       <c r="C63">
         <v>5.6669999999999998</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>5.351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7.2</v>
       </c>
@@ -3214,8 +3178,11 @@
       <c r="C64">
         <v>5.556</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>5.2469999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7.3</v>
       </c>
@@ -3225,8 +3192,11 @@
       <c r="C65">
         <v>5.444</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7.4</v>
       </c>
@@ -3236,8 +3206,11 @@
       <c r="C66">
         <v>5.3330000000000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7.5</v>
       </c>
@@ -3247,8 +3220,11 @@
       <c r="C67">
         <v>5.2220000000000004</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7.6</v>
       </c>
@@ -3258,8 +3234,11 @@
       <c r="C68">
         <v>5.1109999999999998</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7.7</v>
       </c>
@@ -3269,8 +3248,11 @@
       <c r="C69">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>7.8</v>
       </c>
@@ -3280,8 +3262,11 @@
       <c r="C70">
         <v>5.4349999999999996</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>5.0469999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7.9</v>
       </c>
@@ -3291,8 +3276,11 @@
       <c r="C71">
         <v>5.87</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>5.1849999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>8</v>
       </c>
@@ -3302,8 +3290,11 @@
       <c r="C72">
         <v>6.3040000000000003</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>5.4139999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8.1</v>
       </c>
@@ -3313,8 +3304,11 @@
       <c r="C73">
         <v>6.7389999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>5.7279999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>8.1999999999999993</v>
       </c>
@@ -3324,8 +3318,11 @@
       <c r="C74">
         <v>7.1740000000000004</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>6.1210000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>8.3000000000000007</v>
       </c>
@@ -3335,8 +3332,11 @@
       <c r="C75">
         <v>7.609</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>6.5869999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>8.4</v>
       </c>
@@ -3346,8 +3346,11 @@
       <c r="C76">
         <v>8.0429999999999993</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>7.117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8.5</v>
       </c>
@@ -3357,8 +3360,11 @@
       <c r="C77">
         <v>8.4779999999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8.6</v>
       </c>
@@ -3368,8 +3374,11 @@
       <c r="C78">
         <v>8.9130000000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>8.3260000000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8.6999999999999993</v>
       </c>
@@ -3379,8 +3388,11 @@
       <c r="C79">
         <v>9.3480000000000008</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>8.9830000000000005</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>8.8000000000000007</v>
       </c>
@@ -3390,8 +3402,11 @@
       <c r="C80">
         <v>9.7829999999999995</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>9.6590000000000007</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>8.9</v>
       </c>
@@ -3401,8 +3416,11 @@
       <c r="C81">
         <v>10.217000000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>10.340999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9</v>
       </c>
@@ -3412,8 +3430,11 @@
       <c r="C82">
         <v>10.651999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>11.016999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9.1</v>
       </c>
@@ -3423,8 +3444,11 @@
       <c r="C83">
         <v>11.087</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>11.673999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>9.1999999999999993</v>
       </c>
@@ -3434,8 +3458,11 @@
       <c r="C84">
         <v>11.522</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9.3000000000000007</v>
       </c>
@@ -3445,8 +3472,11 @@
       <c r="C85">
         <v>11.957000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>12.882999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9.4</v>
       </c>
@@ -3456,8 +3486,11 @@
       <c r="C86">
         <v>12.391</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>13.413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9.5</v>
       </c>
@@ -3467,8 +3500,11 @@
       <c r="C87">
         <v>12.826000000000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>13.879</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>9.6</v>
       </c>
@@ -3478,8 +3514,11 @@
       <c r="C88">
         <v>13.260999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>14.272</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9.6999999999999993</v>
       </c>
@@ -3489,8 +3528,11 @@
       <c r="C89">
         <v>13.696</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>14.586</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9.8000000000000007</v>
       </c>
@@ -3500,8 +3542,11 @@
       <c r="C90">
         <v>14.13</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>14.815</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9.9</v>
       </c>
@@ -3511,8 +3556,11 @@
       <c r="C91">
         <v>14.565</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>14.952999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>10</v>
       </c>
@@ -3522,8 +3570,11 @@
       <c r="C92">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>10.1</v>
       </c>
@@ -3533,8 +3584,11 @@
       <c r="C93">
         <v>14.63</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>14.909000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>10.199999999999999</v>
       </c>
@@ -3544,8 +3598,11 @@
       <c r="C94">
         <v>14.26</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>14.647</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>10.3</v>
       </c>
@@ -3555,8 +3612,11 @@
       <c r="C95">
         <v>13.89</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>14.237</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>10.4</v>
       </c>
@@ -3566,8 +3626,11 @@
       <c r="C96">
         <v>13.52</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>13.722</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>10.5</v>
       </c>
@@ -3577,8 +3640,11 @@
       <c r="C97">
         <v>13.15</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>13.15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>10.6</v>
       </c>
@@ -3588,8 +3654,11 @@
       <c r="C98">
         <v>12.78</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>12.577999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>10.7</v>
       </c>
@@ -3599,8 +3668,11 @@
       <c r="C99">
         <v>12.41</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>12.063000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>10.8</v>
       </c>
@@ -3610,8 +3682,11 @@
       <c r="C100">
         <v>12.04</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>11.653</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10.9</v>
       </c>
@@ -3621,8 +3696,11 @@
       <c r="C101">
         <v>11.67</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>11.391</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>11</v>
       </c>
@@ -3630,6 +3708,9 @@
         <v>11.3</v>
       </c>
       <c r="C102">
+        <v>11.3</v>
+      </c>
+      <c r="D102">
         <v>11.3</v>
       </c>
     </row>
@@ -3640,6 +3721,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004C6E26232CA7D14687DBD1CB9901E874" ma:contentTypeVersion="6" ma:contentTypeDescription="Ustvari nov dokument." ma:contentTypeScope="" ma:versionID="041837fc78560f70ed22b23f56737390">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1ada11a4-e086-4ab0-84a8-4a21e8af57e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f68be7e90c0f5acbb7f1efdf89eb1597" ns3:_="">
     <xsd:import namespace="1ada11a4-e086-4ab0-84a8-4a21e8af57e8"/>
@@ -3797,22 +3893,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA9E2D8F-BB2D-43F9-82FF-D6269CD5C93B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1ada11a4-e086-4ab0-84a8-4a21e8af57e8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29482C8F-ECCE-41AD-BDF9-BAB7B02F8482}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00BE6CEC-A56E-407D-A162-829C4EBDC690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3828,28 +3933,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29482C8F-ECCE-41AD-BDF9-BAB7B02F8482}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA9E2D8F-BB2D-43F9-82FF-D6269CD5C93B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1ada11a4-e086-4ab0-84a8-4a21e8af57e8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>